<commit_message>
-3.4 nao completo -3.5 start nao completo
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Universidade\2º Ano\2semestre\ATD\ATD20212022-Projeto\Projeto-ATD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7D78AC-6859-47D9-A1C9-3448F2D3B702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A734757-A42A-4CAA-BAFE-88E96E39222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Walk</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>Mean</t>
+  </si>
+  <si>
+    <t>DINAMICAS</t>
+  </si>
+  <si>
+    <t>ESTATICAS</t>
+  </si>
+  <si>
+    <t>TRANSICAO</t>
+  </si>
+  <si>
+    <t>DONT NEED</t>
   </si>
 </sst>
 </file>
@@ -463,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,8 +502,11 @@
       <c r="P1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -532,7 +547,7 @@
         <v>1.6959</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -573,7 +588,7 @@
         <v>1.6470500000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -611,7 +626,7 @@
         <v>2.89005</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
         <v>11</v>
       </c>
@@ -626,18 +641,24 @@
         <v>0.93635000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
       </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
       <c r="M7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -678,7 +699,7 @@
         <v>0.39605000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -716,7 +737,7 @@
         <v>0.89215</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -754,7 +775,7 @@
         <v>2.7057500000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>19</v>
       </c>
@@ -782,7 +803,7 @@
         <v>0.34955000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -792,8 +813,11 @@
       <c r="M13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -834,7 +858,7 @@
         <v>0.27565000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -875,7 +899,7 @@
         <v>0.27565000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>

</xml_diff>